<commit_message>
modify spec for algieba
</commit_message>
<xml_diff>
--- a/algieba/test/system_spec.xlsx
+++ b/algieba/test/system_spec.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15780" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="正常系" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="184">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -1054,10 +1054,6 @@
   </si>
   <si>
     <t>account_type=income</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>date=1000-01-01</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1351,30 +1347,6 @@
   </si>
   <si>
     <t>accounts: {
-  account_type: 'expense',
-  date: '1000-01-01',
-  category: 'システムテスト用データ',
-  price: 100
-}</t>
-    <rPh sb="81" eb="82">
-      <t>ヨウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>accounts: {
-  account_type: 'expense',
-  date: '1000-01-01',
-  content: 'システムテスト用データ',
-  price: 100
-}</t>
-    <rPh sb="73" eb="84">
-      <t>システム</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>accounts: {
   account_type: 'income', 
   date: '1000-01-01',
   content: 'システムテスト用データ',
@@ -1478,15 +1450,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>condition: {
-  price: -1
-}
-with: {
-  account_type: 'expensee'
-}</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>with: {account_type: 'invalid_type'}</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1570,81 +1533,6 @@
     <rPh sb="3" eb="4">
       <t>ミ</t>
     </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_date}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_content}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_category}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_date},
-  {error_code: absent_params_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_account_type},
-  {error_code: absent_params_date},
-  {error_code: absent_params_content},
-  {error_code: absent_params_category},
-  {error_code: absent_params_price}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: absent_params_accounts}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_params_account_type}
-]</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>status: bad_request
-body: [
-  {error_code: invalid_params_account_type}
-]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1661,89 +1549,192 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>date=1000-01-01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>accounts: {
+  account_type: 'income',
+  date: '1000-01-01',
+  category: 'システムテスト用データ',
+  price: 100
+}</t>
+    <rPh sb="80" eb="81">
+      <t>ヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>accounts: {
+  account_type: 'income',
+  date: '1000-01-01',
+  content: 'システムテスト用データ',
+  price: 100
+}</t>
+    <rPh sb="72" eb="83">
+      <t>システム</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>condition: {
+  price: -1
+}
+with: {
+  account_type: 'expense'
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_account_type},
-  {error_code: invalid_params_price}
+  {error_code: absent_param_account_type}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_date}
+  {error_code: absent_param_date}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_price}
+  {error_code: absent_param_content}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_price}
+  {error_code: absent_param_category}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_account_type}
+  {error_code: absent_param_price}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_date}
+  {error_code: absent_param_date},
+  {error_code: absent_param_price}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_date}
+  {error_code: absent_param_account_type},
+  {error_code: absent_param_date},
+  {error_code: absent_param_content},
+  {error_code: absent_param_category},
+  {error_code: absent_param_price}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_account_type},
-  {error_code: invalid_params_date},
-  {error_code: invalid_params_price}
+  {error_code: absent_param_accounts}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: absent_params_with}
+  {error_code: invalid_value_account_type}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_account_type}
+  {error_code: invalid_value_date}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: invalid_params_interval}
+  {error_code: invalid_value_price}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>status: bad_request
 body: [
-  {error_code: absent_params_interval}
+  {error_code: invalid_value_account_type},
+  {error_code: invalid_value_price}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_date}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_price}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_account_type}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_account_type}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_with},
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: absent_param_with}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_account_type}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: invalid_value_interval}
+]</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>status: bad_request
+body: [
+  {error_code: absent_param_interval}
 ]</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2916,7 +2907,7 @@
   <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2973,7 +2964,7 @@
         <v>91</v>
       </c>
       <c r="H3" s="49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="31">
@@ -2996,7 +2987,7 @@
         <v>80</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="31">
@@ -3013,13 +3004,13 @@
         <v>76</v>
       </c>
       <c r="F5" s="28" t="s">
-        <v>93</v>
+        <v>159</v>
       </c>
       <c r="G5" s="28" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="31">
@@ -3036,13 +3027,13 @@
         <v>76</v>
       </c>
       <c r="F6" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="29" t="s">
         <v>53</v>
       </c>
       <c r="H6" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="31">
@@ -3059,13 +3050,13 @@
         <v>76</v>
       </c>
       <c r="F7" s="29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G7" s="29" t="s">
         <v>53</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="31">
@@ -3082,13 +3073,13 @@
         <v>76</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G8" s="29" t="s">
         <v>53</v>
       </c>
       <c r="H8" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="31">
@@ -3105,13 +3096,13 @@
         <v>76</v>
       </c>
       <c r="F9" s="33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G9" s="30" t="s">
         <v>53</v>
       </c>
       <c r="H9" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="31">
@@ -3134,7 +3125,7 @@
         <v>54</v>
       </c>
       <c r="H10" s="45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="83">
@@ -3154,10 +3145,10 @@
         <v>53</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="83">
@@ -3177,10 +3168,10 @@
         <v>56</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="83">
@@ -3200,10 +3191,10 @@
         <v>53</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="83">
@@ -3223,10 +3214,10 @@
         <v>56</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="83">
@@ -3246,10 +3237,10 @@
         <v>53</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H15" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="96">
@@ -3269,10 +3260,10 @@
         <v>57</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="44">
@@ -3292,10 +3283,10 @@
         <v>53</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H17" s="45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="83">
@@ -3315,10 +3306,10 @@
         <v>53</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="83">
@@ -3338,10 +3329,10 @@
         <v>56</v>
       </c>
       <c r="G19" s="33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H19" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="83">
@@ -3361,10 +3352,10 @@
         <v>53</v>
       </c>
       <c r="G20" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H20" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="83">
@@ -3384,10 +3375,10 @@
         <v>53</v>
       </c>
       <c r="G21" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H21" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="96">
@@ -3407,10 +3398,10 @@
         <v>53</v>
       </c>
       <c r="G22" s="33" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H22" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="57">
@@ -3430,10 +3421,10 @@
         <v>58</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" s="47" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -3453,10 +3444,10 @@
         <v>53</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H24" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25" spans="2:8">
@@ -3476,10 +3467,10 @@
         <v>53</v>
       </c>
       <c r="G25" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H25" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="2:8">
@@ -3499,10 +3490,10 @@
         <v>53</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H26" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="2:8">
@@ -3522,10 +3513,10 @@
         <v>59</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H27" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="2:8">
@@ -3545,10 +3536,10 @@
         <v>60</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H28" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="2:8">
@@ -3568,10 +3559,10 @@
         <v>53</v>
       </c>
       <c r="G29" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30" spans="2:8">
@@ -3591,10 +3582,10 @@
         <v>63</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="31">
@@ -3605,19 +3596,19 @@
         <v>6</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E31" s="30" t="s">
         <v>61</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G31" s="30" t="s">
         <v>64</v>
       </c>
       <c r="H31" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="31">
@@ -3628,19 +3619,19 @@
         <v>6</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E32" s="30" t="s">
         <v>61</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G32" s="30" t="s">
         <v>53</v>
       </c>
       <c r="H32" s="47" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="2:8" ht="32" thickBot="1">
@@ -3663,7 +3654,7 @@
         <v>53</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3682,8 +3673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -3736,10 +3727,10 @@
         <v>53</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="83">
@@ -3759,10 +3750,10 @@
         <v>53</v>
       </c>
       <c r="G4" s="43" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="45" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="83">
@@ -3782,10 +3773,10 @@
         <v>69</v>
       </c>
       <c r="G5" s="52" t="s">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="H5" s="46" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="83">
@@ -3805,10 +3796,10 @@
         <v>53</v>
       </c>
       <c r="G6" s="52" t="s">
-        <v>130</v>
+        <v>161</v>
       </c>
       <c r="H6" s="46" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="83">
@@ -3828,10 +3819,10 @@
         <v>53</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H7" s="46" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="70">
@@ -3851,10 +3842,10 @@
         <v>53</v>
       </c>
       <c r="G8" s="52" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="109">
@@ -3874,10 +3865,10 @@
         <v>70</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H9" s="46" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="57">
@@ -3885,22 +3876,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F10" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H10" s="46" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="96">
@@ -3920,10 +3911,10 @@
         <v>53</v>
       </c>
       <c r="G11" s="43" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H11" s="45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="96">
@@ -3943,10 +3934,10 @@
         <v>71</v>
       </c>
       <c r="G12" s="43" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H12" s="45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="96">
@@ -3966,10 +3957,10 @@
         <v>70</v>
       </c>
       <c r="G13" s="43" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H13" s="45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="96">
@@ -3989,10 +3980,10 @@
         <v>72</v>
       </c>
       <c r="G14" s="43" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="H14" s="45" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="57">
@@ -4009,7 +4000,7 @@
         <v>76</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>53</v>
@@ -4032,13 +4023,13 @@
         <v>76</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G16" s="36" t="s">
         <v>73</v>
       </c>
       <c r="H16" s="45" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="57">
@@ -4055,7 +4046,7 @@
         <v>76</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>53</v>
@@ -4081,7 +4072,7 @@
         <v>53</v>
       </c>
       <c r="G18" s="43" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H18" s="45" t="s">
         <v>177</v>
@@ -4104,10 +4095,10 @@
         <v>74</v>
       </c>
       <c r="G19" s="43" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H19" s="45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="83">
@@ -4127,7 +4118,7 @@
         <v>75</v>
       </c>
       <c r="G20" s="43" t="s">
-        <v>144</v>
+        <v>162</v>
       </c>
       <c r="H20" s="45" t="s">
         <v>176</v>
@@ -4150,10 +4141,10 @@
         <v>53</v>
       </c>
       <c r="G21" s="36" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H21" s="45" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="57">
@@ -4173,10 +4164,10 @@
         <v>53</v>
       </c>
       <c r="G22" s="36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H22" s="45" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="57">
@@ -4196,13 +4187,13 @@
         <v>53</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H23" s="45" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="83">
+    <row r="24" spans="2:8" ht="57">
       <c r="B24" s="13">
         <v>22</v>
       </c>
@@ -4219,10 +4210,10 @@
         <v>70</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="H24" s="45" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="57">
@@ -4230,22 +4221,22 @@
         <v>23</v>
       </c>
       <c r="C25" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="G25" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>153</v>
-      </c>
       <c r="H25" s="45" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="57">
@@ -4265,10 +4256,10 @@
         <v>53</v>
       </c>
       <c r="G26" s="36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H26" s="45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="57">
@@ -4288,10 +4279,10 @@
         <v>53</v>
       </c>
       <c r="G27" s="36" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="H27" s="45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="57">
@@ -4311,7 +4302,7 @@
         <v>53</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H28" s="45" t="s">
         <v>176</v>
@@ -4322,22 +4313,22 @@
         <v>27</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>49</v>
       </c>
       <c r="E29" s="37" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F29" s="37" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H29" s="47" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="58" thickBot="1">
@@ -4348,7 +4339,7 @@
         <v>6</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E30" s="37" t="s">
         <v>61</v>
@@ -4360,7 +4351,7 @@
         <v>53</v>
       </c>
       <c r="H30" s="47" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="2:8">

</xml_diff>